<commit_message>
dia de entrega automata y tablas
</commit_message>
<xml_diff>
--- a/estados y funciones.xlsx
+++ b/estados y funciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosVSC\compC\compilador2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37AE1AE7-7F2E-4FEC-9F32-80F0FFAC873E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ED006A-2301-4899-A5D1-50CF06ED8154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5ED76320-F0B9-4B22-8176-03AB80A47559}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>tabla de estados</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -508,20 +511,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC0FD53-9A06-46A9-9497-8DB3FB2B57A4}">
-  <dimension ref="B2:Z20"/>
+  <dimension ref="B2:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>18</v>
       </c>
@@ -594,96 +597,1365 @@
       <c r="Z3" t="s">
         <v>41</v>
       </c>
+      <c r="AA3" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+      <c r="T4">
+        <v>-1</v>
+      </c>
       <c r="U4">
         <v>12</v>
       </c>
+      <c r="V4">
+        <v>14</v>
+      </c>
+      <c r="W4">
+        <v>15</v>
+      </c>
+      <c r="X4">
+        <v>-1</v>
+      </c>
+      <c r="Y4">
+        <v>-1</v>
+      </c>
+      <c r="Z4">
+        <v>16</v>
+      </c>
+      <c r="AA4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="L5">
+        <v>-1</v>
+      </c>
+      <c r="M5">
+        <v>-1</v>
+      </c>
+      <c r="N5">
+        <v>-1</v>
+      </c>
+      <c r="O5">
+        <v>-1</v>
+      </c>
+      <c r="P5">
+        <v>-1</v>
+      </c>
+      <c r="Q5">
+        <v>-1</v>
+      </c>
+      <c r="R5">
+        <v>-1</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+      <c r="U5">
+        <v>-1</v>
+      </c>
+      <c r="V5">
+        <v>-1</v>
+      </c>
+      <c r="W5">
+        <v>-1</v>
+      </c>
+      <c r="X5">
+        <v>-1</v>
+      </c>
+      <c r="Y5">
+        <v>-1</v>
+      </c>
+      <c r="Z5">
+        <v>-1</v>
+      </c>
+      <c r="AA5">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
+      </c>
+      <c r="I6">
+        <v>-1</v>
+      </c>
+      <c r="J6">
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>-1</v>
+      </c>
+      <c r="M6">
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <v>-1</v>
+      </c>
+      <c r="O6">
+        <v>-1</v>
+      </c>
+      <c r="P6">
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <v>-1</v>
+      </c>
+      <c r="R6">
+        <v>-1</v>
+      </c>
+      <c r="S6">
+        <v>-1</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+      <c r="U6">
+        <v>-1</v>
+      </c>
+      <c r="V6">
+        <v>-1</v>
+      </c>
+      <c r="W6">
+        <v>-1</v>
+      </c>
+      <c r="X6">
+        <v>-1</v>
+      </c>
+      <c r="Y6">
+        <v>-1</v>
+      </c>
+      <c r="Z6">
+        <v>-1</v>
+      </c>
+      <c r="AA6">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
+      </c>
+      <c r="M7">
+        <v>-1</v>
+      </c>
+      <c r="N7">
+        <v>-1</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
+      </c>
+      <c r="P7">
+        <v>-1</v>
+      </c>
+      <c r="Q7">
+        <v>-1</v>
+      </c>
+      <c r="R7">
+        <v>-1</v>
+      </c>
+      <c r="S7">
+        <v>-1</v>
+      </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
+      <c r="U7">
+        <v>-1</v>
+      </c>
+      <c r="V7">
+        <v>-1</v>
+      </c>
+      <c r="W7">
+        <v>-1</v>
+      </c>
+      <c r="X7">
+        <v>-1</v>
+      </c>
+      <c r="Y7">
+        <v>-1</v>
+      </c>
+      <c r="Z7">
+        <v>-1</v>
+      </c>
+      <c r="AA7">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="I8">
+        <v>-1</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <v>-1</v>
+      </c>
+      <c r="O8">
+        <v>-1</v>
+      </c>
+      <c r="P8">
+        <v>-1</v>
+      </c>
+      <c r="Q8">
+        <v>-1</v>
+      </c>
+      <c r="R8">
+        <v>-1</v>
+      </c>
+      <c r="S8">
+        <v>-1</v>
+      </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
+      <c r="U8">
+        <v>-1</v>
+      </c>
+      <c r="V8">
+        <v>-1</v>
+      </c>
+      <c r="W8">
+        <v>-1</v>
+      </c>
+      <c r="X8">
+        <v>-1</v>
+      </c>
+      <c r="Y8">
+        <v>-1</v>
+      </c>
+      <c r="Z8">
+        <v>-1</v>
+      </c>
+      <c r="AA8">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>-1</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+      <c r="J9">
+        <v>-1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <v>-1</v>
+      </c>
+      <c r="M9">
+        <v>-1</v>
+      </c>
+      <c r="N9">
+        <v>-1</v>
+      </c>
+      <c r="O9">
+        <v>-1</v>
+      </c>
+      <c r="P9">
+        <v>-1</v>
+      </c>
+      <c r="Q9">
+        <v>-1</v>
+      </c>
+      <c r="R9">
+        <v>-1</v>
+      </c>
+      <c r="S9">
+        <v>-1</v>
+      </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
+      <c r="U9">
+        <v>-1</v>
+      </c>
+      <c r="V9">
+        <v>-1</v>
+      </c>
+      <c r="W9">
+        <v>-1</v>
+      </c>
+      <c r="X9">
+        <v>-1</v>
+      </c>
+      <c r="Y9">
+        <v>-1</v>
+      </c>
+      <c r="Z9">
+        <v>-1</v>
+      </c>
+      <c r="AA9">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+      <c r="I10">
+        <v>-1</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>-1</v>
+      </c>
+      <c r="N10">
+        <v>-1</v>
+      </c>
+      <c r="O10">
+        <v>-1</v>
+      </c>
+      <c r="P10">
+        <v>-1</v>
+      </c>
+      <c r="Q10">
+        <v>-1</v>
+      </c>
+      <c r="R10">
+        <v>-1</v>
+      </c>
+      <c r="S10">
+        <v>-1</v>
+      </c>
+      <c r="T10">
+        <v>-1</v>
+      </c>
+      <c r="U10">
+        <v>-1</v>
+      </c>
+      <c r="V10">
+        <v>-1</v>
+      </c>
+      <c r="W10">
+        <v>-1</v>
+      </c>
+      <c r="X10">
+        <v>-1</v>
+      </c>
+      <c r="Y10">
+        <v>-1</v>
+      </c>
+      <c r="Z10">
+        <v>-1</v>
+      </c>
+      <c r="AA10">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <v>-1</v>
+      </c>
+      <c r="H11">
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <v>-1</v>
+      </c>
+      <c r="J11">
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+      <c r="L11">
+        <v>-1</v>
+      </c>
+      <c r="M11">
+        <v>-1</v>
+      </c>
+      <c r="N11">
+        <v>-1</v>
+      </c>
+      <c r="O11">
+        <v>-1</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
+      </c>
+      <c r="Q11">
+        <v>-1</v>
+      </c>
+      <c r="R11">
+        <v>-1</v>
+      </c>
+      <c r="S11">
+        <v>-1</v>
+      </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
+      <c r="U11">
+        <v>-1</v>
+      </c>
+      <c r="V11">
+        <v>-1</v>
+      </c>
+      <c r="W11">
+        <v>-1</v>
+      </c>
+      <c r="X11">
+        <v>-1</v>
+      </c>
+      <c r="Y11">
+        <v>-1</v>
+      </c>
+      <c r="Z11">
+        <v>-1</v>
+      </c>
+      <c r="AA11">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>-1</v>
+      </c>
+      <c r="H12">
+        <v>-1</v>
+      </c>
+      <c r="I12">
+        <v>-1</v>
+      </c>
+      <c r="J12">
+        <v>-1</v>
+      </c>
+      <c r="K12">
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
+      </c>
+      <c r="M12">
+        <v>-1</v>
+      </c>
+      <c r="N12">
+        <v>-1</v>
+      </c>
+      <c r="O12">
+        <v>-1</v>
+      </c>
+      <c r="P12">
+        <v>-1</v>
+      </c>
+      <c r="Q12">
+        <v>-1</v>
+      </c>
+      <c r="R12">
+        <v>-1</v>
+      </c>
+      <c r="S12">
+        <v>-1</v>
+      </c>
+      <c r="T12">
+        <v>-1</v>
+      </c>
+      <c r="U12">
+        <v>-1</v>
+      </c>
+      <c r="V12">
+        <v>-1</v>
+      </c>
+      <c r="W12">
+        <v>-1</v>
+      </c>
+      <c r="X12">
+        <v>-1</v>
+      </c>
+      <c r="Y12">
+        <v>-1</v>
+      </c>
+      <c r="Z12">
+        <v>-1</v>
+      </c>
+      <c r="AA12">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="H13">
+        <v>-1</v>
+      </c>
+      <c r="I13">
+        <v>-1</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
+      <c r="K13">
+        <v>-1</v>
+      </c>
+      <c r="L13">
+        <v>-1</v>
+      </c>
+      <c r="M13">
+        <v>-1</v>
+      </c>
+      <c r="N13">
+        <v>-1</v>
+      </c>
+      <c r="O13">
+        <v>-1</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
+      </c>
+      <c r="Q13">
+        <v>-1</v>
+      </c>
+      <c r="R13">
+        <v>-1</v>
+      </c>
+      <c r="S13">
+        <v>-1</v>
+      </c>
+      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="V13">
+        <v>-1</v>
+      </c>
+      <c r="W13">
+        <v>-1</v>
+      </c>
+      <c r="X13">
+        <v>-1</v>
+      </c>
+      <c r="Y13">
+        <v>-1</v>
+      </c>
+      <c r="Z13">
+        <v>-1</v>
+      </c>
+      <c r="AA13">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>10</v>
+      </c>
+      <c r="T14">
+        <v>11</v>
+      </c>
+      <c r="U14">
+        <v>10</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
+      </c>
+      <c r="X14">
+        <v>10</v>
+      </c>
+      <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14">
+        <v>10</v>
+      </c>
+      <c r="AA14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>10</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="V15">
+        <v>10</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15">
+        <v>10</v>
+      </c>
+      <c r="Y15">
+        <v>10</v>
+      </c>
+      <c r="Z15">
+        <v>10</v>
+      </c>
+      <c r="AA15">
+        <v>10</v>
+      </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <v>-1</v>
+      </c>
+      <c r="H16">
+        <v>-1</v>
+      </c>
+      <c r="I16">
+        <v>-1</v>
+      </c>
+      <c r="J16">
+        <v>-1</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+      <c r="L16">
+        <v>-1</v>
+      </c>
+      <c r="M16">
+        <v>-1</v>
+      </c>
+      <c r="N16">
+        <v>-1</v>
+      </c>
+      <c r="O16">
+        <v>-1</v>
+      </c>
+      <c r="P16">
+        <v>-1</v>
+      </c>
+      <c r="Q16">
+        <v>-1</v>
+      </c>
+      <c r="R16">
+        <v>-1</v>
+      </c>
+      <c r="S16">
+        <v>-1</v>
+      </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
       <c r="U16">
         <v>13</v>
       </c>
+      <c r="V16">
+        <v>-1</v>
+      </c>
+      <c r="W16">
+        <v>-1</v>
+      </c>
+      <c r="X16">
+        <v>-1</v>
+      </c>
+      <c r="Y16">
+        <v>-1</v>
+      </c>
+      <c r="Z16">
+        <v>-1</v>
+      </c>
+      <c r="AA16">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>-1</v>
+      </c>
+      <c r="G17">
+        <v>-1</v>
+      </c>
+      <c r="H17">
+        <v>-1</v>
+      </c>
+      <c r="I17">
+        <v>-1</v>
+      </c>
+      <c r="J17">
+        <v>-1</v>
+      </c>
+      <c r="K17">
+        <v>-1</v>
+      </c>
+      <c r="L17">
+        <v>-1</v>
+      </c>
+      <c r="M17">
+        <v>-1</v>
+      </c>
+      <c r="N17">
+        <v>-1</v>
+      </c>
+      <c r="O17">
+        <v>-1</v>
+      </c>
+      <c r="P17">
+        <v>-1</v>
+      </c>
+      <c r="Q17">
+        <v>-1</v>
+      </c>
+      <c r="R17">
+        <v>-1</v>
+      </c>
+      <c r="S17">
+        <v>-1</v>
+      </c>
+      <c r="T17">
+        <v>-1</v>
+      </c>
+      <c r="U17">
+        <v>-1</v>
+      </c>
+      <c r="V17">
+        <v>-1</v>
+      </c>
+      <c r="W17">
+        <v>-1</v>
+      </c>
+      <c r="X17">
+        <v>-1</v>
+      </c>
+      <c r="Y17">
+        <v>-1</v>
+      </c>
+      <c r="Z17">
+        <v>-1</v>
+      </c>
+      <c r="AA17">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>15</v>
       </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>-1</v>
+      </c>
+      <c r="G18">
+        <v>-1</v>
+      </c>
+      <c r="H18">
+        <v>-1</v>
+      </c>
+      <c r="I18">
+        <v>-1</v>
+      </c>
+      <c r="J18">
+        <v>-1</v>
+      </c>
+      <c r="K18">
+        <v>-1</v>
+      </c>
+      <c r="L18">
+        <v>-1</v>
+      </c>
+      <c r="M18">
+        <v>-1</v>
+      </c>
+      <c r="N18">
+        <v>-1</v>
+      </c>
+      <c r="O18">
+        <v>-1</v>
+      </c>
+      <c r="P18">
+        <v>-1</v>
+      </c>
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>-1</v>
+      </c>
+      <c r="S18">
+        <v>-1</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+      <c r="U18">
+        <v>-1</v>
+      </c>
+      <c r="V18">
+        <v>-1</v>
+      </c>
+      <c r="W18">
+        <v>-1</v>
+      </c>
+      <c r="X18">
+        <v>-1</v>
+      </c>
+      <c r="Y18">
+        <v>-1</v>
+      </c>
+      <c r="Z18">
+        <v>-1</v>
+      </c>
+      <c r="AA18">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>16</v>
       </c>
+      <c r="C19">
+        <v>-1</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>-1</v>
+      </c>
+      <c r="I19">
+        <v>-1</v>
+      </c>
+      <c r="J19">
+        <v>-1</v>
+      </c>
+      <c r="K19">
+        <v>-1</v>
+      </c>
+      <c r="L19">
+        <v>-1</v>
+      </c>
+      <c r="M19">
+        <v>-1</v>
+      </c>
+      <c r="N19">
+        <v>-1</v>
+      </c>
+      <c r="O19">
+        <v>-1</v>
+      </c>
+      <c r="P19">
+        <v>-1</v>
+      </c>
+      <c r="Q19">
+        <v>-1</v>
+      </c>
+      <c r="R19">
+        <v>-1</v>
+      </c>
+      <c r="S19">
+        <v>-1</v>
+      </c>
+      <c r="T19">
+        <v>-1</v>
+      </c>
+      <c r="U19">
+        <v>-1</v>
+      </c>
+      <c r="V19">
+        <v>-1</v>
+      </c>
+      <c r="W19">
+        <v>-1</v>
+      </c>
+      <c r="X19">
+        <v>-1</v>
+      </c>
+      <c r="Y19">
+        <v>-1</v>
+      </c>
+      <c r="Z19">
+        <v>-1</v>
+      </c>
+      <c r="AA19">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+      <c r="E20">
+        <v>-1</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>-1</v>
+      </c>
+      <c r="H20">
+        <v>-1</v>
+      </c>
+      <c r="I20">
+        <v>-1</v>
+      </c>
+      <c r="J20">
+        <v>-1</v>
+      </c>
+      <c r="K20">
+        <v>-1</v>
+      </c>
+      <c r="L20">
+        <v>-1</v>
+      </c>
+      <c r="M20">
+        <v>-1</v>
+      </c>
+      <c r="N20">
+        <v>-1</v>
+      </c>
+      <c r="O20">
+        <v>-1</v>
+      </c>
+      <c r="P20">
+        <v>-1</v>
+      </c>
+      <c r="Q20">
+        <v>-1</v>
+      </c>
+      <c r="R20">
+        <v>-1</v>
+      </c>
+      <c r="S20">
+        <v>-1</v>
+      </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
+      <c r="U20">
+        <v>-1</v>
+      </c>
+      <c r="V20">
+        <v>-1</v>
+      </c>
+      <c r="W20">
+        <v>-1</v>
+      </c>
+      <c r="X20">
+        <v>-1</v>
+      </c>
+      <c r="Y20">
+        <v>-1</v>
+      </c>
+      <c r="Z20">
+        <v>-1</v>
+      </c>
+      <c r="AA20">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregado de corchetes a "TOKENS"
</commit_message>
<xml_diff>
--- a/estados y funciones.xlsx
+++ b/estados y funciones.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosVSC\compC\compilador2021\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ED006A-2301-4899-A5D1-50CF06ED8154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5ED76320-F0B9-4B22-8176-03AB80A47559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -159,8 +153,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -309,7 +303,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -503,28 +497,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC0FD53-9A06-46A9-9497-8DB3FB2B57A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27">
       <c r="C3" t="s">
         <v>18</v>
       </c>
@@ -601,7 +595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -681,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -761,7 +755,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -841,7 +835,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -921,7 +915,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1001,7 +995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1155,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1235,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1321,7 +1315,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1379,6 +1373,9 @@
       <c r="T13">
         <v>10</v>
       </c>
+      <c r="U13">
+        <v>-1</v>
+      </c>
       <c r="V13">
         <v>-1</v>
       </c>
@@ -1398,7 +1395,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1478,7 +1475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1635,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1715,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27">
       <c r="B20" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
1er Punto de Control
</commit_message>
<xml_diff>
--- a/estados y funciones.xlsx
+++ b/estados y funciones.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosVSC\compilador2021\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A72DC1-9BEB-4C7B-90A1-D10203311595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1905" windowWidth="15375" windowHeight="8325"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -345,8 +351,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,27 +866,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T75" sqref="T75"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:27" ht="19.5" thickBot="1">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -911,7 +917,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="19.5" thickBot="1">
+    <row r="3" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
@@ -988,7 +994,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="19.5" thickBot="1">
+    <row r="4" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -1067,7 +1073,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="19.5" thickBot="1">
+    <row r="5" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
@@ -1078,8 +1084,8 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>50</v>
+      <c r="E5" s="7">
+        <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>50</v>
@@ -1146,7 +1152,7 @@
       </c>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="19.5" thickBot="1">
+    <row r="6" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
@@ -1225,7 +1231,7 @@
       </c>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="19.5" thickBot="1">
+    <row r="7" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -1304,7 +1310,7 @@
       </c>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="19.5" thickBot="1">
+    <row r="8" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -1383,7 +1389,7 @@
       </c>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="19.5" thickBot="1">
+    <row r="9" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -1462,7 +1468,7 @@
       </c>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" ht="19.5" thickBot="1">
+    <row r="10" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
         <v>7</v>
@@ -1541,7 +1547,7 @@
       </c>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="19.5" thickBot="1">
+    <row r="11" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1620,7 +1626,7 @@
       </c>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="19.5" thickBot="1">
+    <row r="12" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
         <v>9</v>
@@ -1699,7 +1705,7 @@
       </c>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="19.5" thickBot="1">
+    <row r="13" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
@@ -1778,7 +1784,7 @@
       </c>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="19.5" thickBot="1">
+    <row r="14" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -1790,7 +1796,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="7">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="F14" s="7">
         <v>9</v>
@@ -1857,7 +1863,7 @@
       </c>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="19.5" thickBot="1">
+    <row r="15" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>12</v>
@@ -1936,7 +1942,7 @@
       </c>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="19.5" thickBot="1">
+    <row r="16" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>13</v>
@@ -2015,7 +2021,7 @@
       </c>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="19.5" thickBot="1">
+    <row r="17" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
@@ -2094,7 +2100,7 @@
       </c>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="19.5" thickBot="1">
+    <row r="18" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
         <v>15</v>
@@ -2173,7 +2179,7 @@
       </c>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="19.5" thickBot="1">
+    <row r="19" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
         <v>16</v>
@@ -2252,7 +2258,7 @@
       </c>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="19.5" thickBot="1">
+    <row r="20" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
         <v>17</v>
@@ -2331,7 +2337,7 @@
       </c>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="19.5" thickBot="1">
+    <row r="21" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
@@ -2339,8 +2345,8 @@
       <c r="C21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="7">
-        <v>-1</v>
+      <c r="D21" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>50</v>
@@ -2410,7 +2416,7 @@
       </c>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="19.5" thickBot="1">
+    <row r="22" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
         <v>39</v>
@@ -2489,7 +2495,7 @@
       </c>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="19.5" thickBot="1">
+    <row r="23" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
         <v>40</v>
@@ -2568,7 +2574,7 @@
       </c>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="19.5" thickBot="1">
+    <row r="24" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
         <v>41</v>
@@ -2647,7 +2653,7 @@
       </c>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="19.5" thickBot="1">
+    <row r="25" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
         <v>42</v>
@@ -2726,7 +2732,7 @@
       </c>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="19.5" thickBot="1">
+    <row r="26" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
         <v>43</v>
@@ -2805,7 +2811,7 @@
       </c>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="19.5" thickBot="1">
+    <row r="27" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
         <v>44</v>
@@ -2884,7 +2890,7 @@
       </c>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="19.5" thickBot="1">
+    <row r="28" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="5" t="s">
         <v>45</v>
@@ -2963,7 +2969,7 @@
       </c>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="1:27" ht="19.5" thickBot="1">
+    <row r="29" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="5" t="s">
         <v>46</v>
@@ -3042,7 +3048,7 @@
       </c>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="19.5" thickBot="1">
+    <row r="30" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="5" t="s">
         <v>47</v>
@@ -3121,7 +3127,7 @@
       </c>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="19.5" thickBot="1">
+    <row r="31" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
         <v>48</v>
@@ -3200,7 +3206,7 @@
       </c>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" thickBot="1">
+    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3229,7 +3235,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="1:27" ht="15.75" thickBot="1">
+    <row r="33" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3258,7 +3264,7 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" spans="1:27" ht="15.75" thickBot="1">
+    <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3287,7 +3293,7 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" spans="1:27" ht="15.75" thickBot="1">
+    <row r="35" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="11" t="s">
         <v>51</v>
@@ -3318,7 +3324,7 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" spans="1:27" ht="15.75" thickBot="1">
+    <row r="36" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -3347,7 +3353,7 @@
       <c r="Z36" s="12"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="1:27" ht="19.5" thickBot="1">
+    <row r="37" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6" t="s">
@@ -3424,7 +3430,7 @@
       </c>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="1:27" ht="19.5" thickBot="1">
+    <row r="38" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="B38" s="5" t="s">
         <v>56</v>
@@ -3503,7 +3509,7 @@
       </c>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" ht="19.5" thickBot="1">
+    <row r="39" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="5" t="s">
         <v>57</v>
@@ -3582,7 +3588,7 @@
       </c>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:27" ht="19.5" thickBot="1">
+    <row r="40" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="B40" s="5" t="s">
         <v>52</v>
@@ -3661,7 +3667,7 @@
       </c>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" spans="1:27" ht="19.5" thickBot="1">
+    <row r="41" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
       <c r="B41" s="5" t="s">
         <v>53</v>
@@ -3740,7 +3746,7 @@
       </c>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" spans="1:27" ht="19.5" thickBot="1">
+    <row r="42" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="B42" s="5" t="s">
         <v>54</v>
@@ -3819,7 +3825,7 @@
       </c>
       <c r="AA42" s="1"/>
     </row>
-    <row r="43" spans="1:27" ht="19.5" thickBot="1">
+    <row r="43" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
         <v>55</v>
@@ -3898,7 +3904,7 @@
       </c>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" spans="1:27" ht="19.5" thickBot="1">
+    <row r="44" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="B44" s="5" t="s">
         <v>58</v>
@@ -3977,7 +3983,7 @@
       </c>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" spans="1:27" ht="19.5" thickBot="1">
+    <row r="45" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
       <c r="B45" s="6" t="s">
         <v>63</v>
@@ -4056,7 +4062,7 @@
       </c>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" spans="1:27" ht="19.5" thickBot="1">
+    <row r="46" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="B46" s="6" t="s">
         <v>64</v>
@@ -4135,7 +4141,7 @@
       </c>
       <c r="AA46" s="1"/>
     </row>
-    <row r="47" spans="1:27" ht="19.5" thickBot="1">
+    <row r="47" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
         <v>79</v>
@@ -4214,7 +4220,7 @@
       </c>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" spans="1:27" ht="19.5" thickBot="1">
+    <row r="48" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="B48" s="6" t="s">
         <v>80</v>
@@ -4293,7 +4299,7 @@
       </c>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" spans="1:27" ht="19.5" thickBot="1">
+    <row r="49" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="B49" s="6" t="s">
         <v>65</v>
@@ -4372,7 +4378,7 @@
       </c>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="1:27" ht="19.5" thickBot="1">
+    <row r="50" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="B50" s="6" t="s">
         <v>81</v>
@@ -4451,7 +4457,7 @@
       </c>
       <c r="AA50" s="1"/>
     </row>
-    <row r="51" spans="1:27" ht="19.5" thickBot="1">
+    <row r="51" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="6" t="s">
         <v>66</v>
@@ -4530,7 +4536,7 @@
       </c>
       <c r="AA51" s="1"/>
     </row>
-    <row r="52" spans="1:27" ht="19.5" thickBot="1">
+    <row r="52" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="B52" s="6" t="s">
         <v>67</v>
@@ -4609,7 +4615,7 @@
       </c>
       <c r="AA52" s="1"/>
     </row>
-    <row r="53" spans="1:27" ht="19.5" thickBot="1">
+    <row r="53" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
@@ -4618,77 +4624,77 @@
         <v>50</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="K53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="N53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="Q53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="R53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="S53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="T53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="U53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="V53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="W53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="X53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="Y53" s="13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="Z53" s="14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" spans="1:27" ht="19.5" thickBot="1">
+    <row r="54" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4"/>
       <c r="B54" s="6" t="s">
         <v>69</v>
@@ -4767,7 +4773,7 @@
       </c>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" spans="1:27" ht="19.5" thickBot="1">
+    <row r="55" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="B55" s="6" t="s">
         <v>70</v>
@@ -4846,7 +4852,7 @@
       </c>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" spans="1:27" ht="19.5" thickBot="1">
+    <row r="56" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="B56" s="6" t="s">
         <v>71</v>
@@ -4925,7 +4931,7 @@
       </c>
       <c r="AA56" s="1"/>
     </row>
-    <row r="57" spans="1:27" ht="19.5" thickBot="1">
+    <row r="57" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="B57" s="6" t="s">
         <v>72</v>
@@ -5004,7 +5010,7 @@
       </c>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" spans="1:27" ht="19.5" thickBot="1">
+    <row r="58" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="6" t="s">
         <v>73</v>
@@ -5083,7 +5089,7 @@
       </c>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" spans="1:27" ht="19.5" thickBot="1">
+    <row r="59" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="B59" s="6" t="s">
         <v>74</v>
@@ -5162,7 +5168,7 @@
       </c>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" spans="1:27" ht="19.5" thickBot="1">
+    <row r="60" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="B60" s="6" t="s">
         <v>75</v>
@@ -5241,7 +5247,7 @@
       </c>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" spans="1:27" ht="19.5" thickBot="1">
+    <row r="61" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="6" t="s">
         <v>76</v>
@@ -5320,7 +5326,7 @@
       </c>
       <c r="AA61" s="1"/>
     </row>
-    <row r="62" spans="1:27" ht="19.5" thickBot="1">
+    <row r="62" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="6" t="s">
         <v>77</v>
@@ -5399,7 +5405,7 @@
       </c>
       <c r="AA62" s="1"/>
     </row>
-    <row r="63" spans="1:27" ht="19.5" thickBot="1">
+    <row r="63" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="B63" s="6" t="s">
         <v>78</v>
@@ -5478,7 +5484,7 @@
       </c>
       <c r="AA63" s="1"/>
     </row>
-    <row r="64" spans="1:27" ht="19.5" thickBot="1">
+    <row r="64" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
       <c r="C64" s="13"/>
@@ -5507,7 +5513,7 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="1"/>
     </row>
-    <row r="65" spans="1:27" ht="15.75" thickBot="1">
+    <row r="65" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="12"/>
@@ -5536,7 +5542,7 @@
       <c r="Z65" s="5"/>
       <c r="AA65" s="1"/>
     </row>
-    <row r="66" spans="1:27" ht="15.75" thickBot="1">
+    <row r="66" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -5565,7 +5571,7 @@
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="1:27" ht="15.75" thickBot="1">
+    <row r="67" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -5594,7 +5600,7 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" spans="1:27" ht="15.75" thickBot="1">
+    <row r="68" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="16"/>
       <c r="C68" s="18"/>
@@ -5625,7 +5631,7 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" spans="1:27" ht="15.75" thickBot="1">
+    <row r="69" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="16"/>
       <c r="C69" s="18"/>
@@ -5656,7 +5662,7 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" spans="1:27" ht="15.75" thickBot="1">
+    <row r="70" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="16"/>
       <c r="C70" s="18"/>
@@ -5687,7 +5693,7 @@
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" spans="1:27" ht="15.75" thickBot="1">
+    <row r="71" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="16"/>
       <c r="C71" s="18"/>
@@ -5718,7 +5724,7 @@
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
     </row>
-    <row r="72" spans="1:27" ht="15.75" thickBot="1">
+    <row r="72" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="16"/>
       <c r="C72" s="18"/>
@@ -5749,7 +5755,7 @@
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
     </row>
-    <row r="73" spans="1:27" ht="15.75" thickBot="1">
+    <row r="73" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="16"/>
       <c r="C73" s="18"/>
@@ -5780,7 +5786,7 @@
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
     </row>
-    <row r="74" spans="1:27" ht="15.75" thickBot="1">
+    <row r="74" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="20"/>
@@ -5811,7 +5817,7 @@
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
     </row>
-    <row r="75" spans="1:27" ht="15.75" thickBot="1">
+    <row r="75" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="20"/>
@@ -5842,7 +5848,7 @@
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
     </row>
-    <row r="76" spans="1:27" ht="15.75" thickBot="1">
+    <row r="76" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="20"/>
@@ -5873,7 +5879,7 @@
       <c r="Z76" s="1"/>
       <c r="AA76" s="1"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" thickBot="1">
+    <row r="77" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="20"/>
@@ -5904,7 +5910,7 @@
       <c r="Z77" s="1"/>
       <c r="AA77" s="1"/>
     </row>
-    <row r="78" spans="1:27" ht="15.75" thickBot="1">
+    <row r="78" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="20"/>
@@ -5935,7 +5941,7 @@
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
     </row>
-    <row r="79" spans="1:27" ht="15.75" thickBot="1">
+    <row r="79" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="20"/>
@@ -5966,7 +5972,7 @@
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
     </row>
-    <row r="80" spans="1:27" ht="15.75" thickBot="1">
+    <row r="80" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="20"/>
@@ -5997,7 +6003,7 @@
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>
     </row>
-    <row r="81" spans="1:27" ht="15.75" thickBot="1">
+    <row r="81" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="20"/>
@@ -6026,7 +6032,7 @@
       <c r="Z81" s="1"/>
       <c r="AA81" s="1"/>
     </row>
-    <row r="82" spans="1:27" ht="15.75" thickBot="1">
+    <row r="82" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="20"/>
@@ -6057,7 +6063,7 @@
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
     </row>
-    <row r="83" spans="1:27" ht="15.75" thickBot="1">
+    <row r="83" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="20"/>
@@ -6086,7 +6092,7 @@
       <c r="Z83" s="1"/>
       <c r="AA83" s="1"/>
     </row>
-    <row r="84" spans="1:27" ht="15.75" thickBot="1">
+    <row r="84" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="20"/>
@@ -6117,7 +6123,7 @@
       <c r="Z84" s="1"/>
       <c r="AA84" s="1"/>
     </row>
-    <row r="85" spans="1:27" ht="15.75" thickBot="1">
+    <row r="85" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="20"/>
@@ -6148,7 +6154,7 @@
       <c r="Z85" s="1"/>
       <c r="AA85" s="1"/>
     </row>
-    <row r="86" spans="1:27" ht="15.75" thickBot="1">
+    <row r="86" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="20"/>
@@ -6179,7 +6185,7 @@
       <c r="Z86" s="1"/>
       <c r="AA86" s="1"/>
     </row>
-    <row r="87" spans="1:27" ht="15.75" thickBot="1">
+    <row r="87" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="20"/>
@@ -6210,7 +6216,7 @@
       <c r="Z87" s="1"/>
       <c r="AA87" s="1"/>
     </row>
-    <row r="88" spans="1:27" ht="15.75" thickBot="1">
+    <row r="88" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="20"/>
@@ -6241,7 +6247,7 @@
       <c r="Z88" s="1"/>
       <c r="AA88" s="1"/>
     </row>
-    <row r="89" spans="1:27" ht="15.75" thickBot="1">
+    <row r="89" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="20"/>
@@ -6272,7 +6278,7 @@
       <c r="Z89" s="1"/>
       <c r="AA89" s="1"/>
     </row>
-    <row r="90" spans="1:27" ht="15.75" thickBot="1">
+    <row r="90" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="20"/>
@@ -6303,7 +6309,7 @@
       <c r="Z90" s="1"/>
       <c r="AA90" s="1"/>
     </row>
-    <row r="91" spans="1:27" ht="15.75" thickBot="1">
+    <row r="91" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="20"/>
@@ -6334,7 +6340,7 @@
       <c r="Z91" s="1"/>
       <c r="AA91" s="1"/>
     </row>
-    <row r="92" spans="1:27" ht="15.75" thickBot="1">
+    <row r="92" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="20"/>
@@ -6365,7 +6371,7 @@
       <c r="Z92" s="1"/>
       <c r="AA92" s="1"/>
     </row>
-    <row r="93" spans="1:27" ht="15.75" thickBot="1">
+    <row r="93" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="20"/>
@@ -6396,7 +6402,7 @@
       <c r="Z93" s="1"/>
       <c r="AA93" s="1"/>
     </row>
-    <row r="94" spans="1:27" ht="15.75" thickBot="1">
+    <row r="94" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="20"/>
@@ -6427,7 +6433,7 @@
       <c r="Z94" s="1"/>
       <c r="AA94" s="1"/>
     </row>
-    <row r="95" spans="1:27" ht="15.75" thickBot="1">
+    <row r="95" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="20"/>
@@ -6456,7 +6462,7 @@
       <c r="Z95" s="1"/>
       <c r="AA95" s="1"/>
     </row>
-    <row r="96" spans="1:27" ht="15.75" thickBot="1">
+    <row r="96" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -6489,12 +6495,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
@@ -6507,16 +6517,12 @@
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>